<commit_message>
Created forms for logging in and registering
Forms can be accessed via '/login/' and '/login/register'.
</commit_message>
<xml_diff>
--- a/Team 98 burndown chart.xlsx
+++ b/Team 98 burndown chart.xlsx
@@ -517,7 +517,10 @@
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41</c:v>
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2886,7 +2889,7 @@
   <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3013,7 +3016,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -3021,6 +3024,9 @@
         <v>15</v>
       </c>
       <c r="B18" s="3"/>
+      <c r="C18" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">

</xml_diff>

<commit_message>
Updataed sprint plan and burndown chart
</commit_message>
<xml_diff>
--- a/Team 98 burndown chart.xlsx
+++ b/Team 98 burndown chart.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kurtis Mason\Documents\GitHub\IFB299-SmartCity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\GitHub\IFB299-SmartCity\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burn down chart" sheetId="2" r:id="rId1"/>
@@ -51,8 +51,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -65,6 +65,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -102,15 +107,15 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -143,7 +148,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -551,6 +556,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2915,408 +2923,411 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="29.85546875" style="1"/>
+    <col min="1" max="16384" width="29.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>300</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>2</v>
       </c>
       <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
       <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>20</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>41</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>19</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>18</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>17</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
         <v>15</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>14</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="1">
+      <c r="C19" s="2">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
         <v>13</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="1">
+      <c r="C20" s="2">
         <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>12</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="1">
+      <c r="C21" s="2">
         <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>11</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="1">
+      <c r="C22" s="2">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
         <v>10</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="1">
+      <c r="C23" s="2">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+      <c r="A24" s="2">
         <v>9</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="1">
+      <c r="C24" s="2">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+      <c r="A25" s="2">
         <v>8</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="1">
+      <c r="C25" s="2">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+      <c r="A26" s="2">
         <v>7</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="1">
+      <c r="C26" s="2">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+      <c r="A27" s="2">
         <v>6</v>
       </c>
       <c r="B27" s="3"/>
-      <c r="C27" s="1">
+      <c r="C27" s="2">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+      <c r="A28" s="2">
         <v>5</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="1">
+      <c r="C28" s="2">
         <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
+      <c r="A29" s="2">
         <v>4</v>
       </c>
       <c r="B29" s="3"/>
+      <c r="C29" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
+      <c r="A30" s="2">
         <v>3</v>
       </c>
       <c r="B30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
+      <c r="A31" s="2">
         <v>2</v>
       </c>
       <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
+      <c r="A32" s="2">
         <v>1</v>
       </c>
       <c r="B32" s="3"/>
-      <c r="D32" s="2"/>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
+      <c r="A33" s="2">
         <v>0</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>0</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D34" s="2"/>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D35" s="2"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D37" s="2"/>
+      <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D38" s="2"/>
+      <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D39" s="2"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D40" s="2"/>
+      <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D41" s="2"/>
+      <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D42" s="2"/>
+      <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D43" s="2"/>
+      <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D44" s="2"/>
+      <c r="D44" s="5"/>
     </row>
     <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
+      <c r="A64" s="1"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D66" s="2"/>
+      <c r="D66" s="5"/>
     </row>
     <row r="67" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D67" s="2"/>
+      <c r="D67" s="5"/>
     </row>
     <row r="68" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D68" s="2"/>
+      <c r="D68" s="5"/>
     </row>
     <row r="69" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D69" s="2"/>
+      <c r="D69" s="5"/>
     </row>
     <row r="70" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D70" s="2"/>
+      <c r="D70" s="5"/>
     </row>
     <row r="71" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D71" s="2"/>
+      <c r="D71" s="5"/>
     </row>
     <row r="72" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D72" s="2"/>
+      <c r="D72" s="5"/>
     </row>
     <row r="73" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D73" s="2"/>
+      <c r="D73" s="5"/>
     </row>
     <row r="74" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D74" s="2"/>
+      <c r="D74" s="5"/>
     </row>
     <row r="75" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D75" s="2"/>
+      <c r="D75" s="5"/>
     </row>
     <row r="76" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D76" s="2"/>
+      <c r="D76" s="5"/>
     </row>
     <row r="77" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D77" s="2"/>
+      <c r="D77" s="5"/>
     </row>
     <row r="78" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D78" s="2"/>
+      <c r="D78" s="5"/>
     </row>
     <row r="79" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D79" s="2"/>
+      <c r="D79" s="5"/>
     </row>
     <row r="80" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D80" s="2"/>
+      <c r="D80" s="5"/>
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="4"/>
-      <c r="B101" s="5"/>
-      <c r="C101" s="5"/>
+      <c r="A101" s="1"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="6"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D103" s="2"/>
+      <c r="D103" s="5"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D104" s="2"/>
+      <c r="D104" s="5"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D105" s="2"/>
+      <c r="D105" s="5"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D106" s="2"/>
+      <c r="D106" s="5"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D107" s="2"/>
+      <c r="D107" s="5"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D108" s="2"/>
+      <c r="D108" s="5"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D109" s="2"/>
+      <c r="D109" s="5"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D110" s="2"/>
+      <c r="D110" s="5"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D111" s="2"/>
+      <c r="D111" s="5"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D112" s="2"/>
+      <c r="D112" s="5"/>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D113" s="2"/>
+      <c r="D113" s="5"/>
     </row>
     <row r="114" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D114" s="2"/>
+      <c r="D114" s="5"/>
     </row>
     <row r="115" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D115" s="2"/>
+      <c r="D115" s="5"/>
     </row>
     <row r="116" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D116" s="2"/>
+      <c r="D116" s="5"/>
     </row>
     <row r="117" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D117" s="2"/>
+      <c r="D117" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>